<commit_message>
Refined parts list, did more research into Camarray HATs
</commit_message>
<xml_diff>
--- a/Parts List - Digital Nishika N8000.xlsx
+++ b/Parts List - Digital Nishika N8000.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Price</t>
   </si>
@@ -22,49 +22,145 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Camarray HAT &amp; Cameras</t>
-  </si>
-  <si>
-    <t>https://www.uctronics.com/arducam-12mp-4-imx477-quadrascopic-camera-bundle-kit-raspberry-pi-nvidia-jetson%20nano.html</t>
-  </si>
-  <si>
-    <t>https://www.uctronics.com/camera-modules/camera-for-raspberry-pi/arducam-12mp-imx708-quad-camera-kit-wide-angle-stereo-synchronized-camera-module-for-raspberry-pi.html</t>
+    <t>Camarray HAT &amp; 4 Cameras</t>
+  </si>
+  <si>
+    <t>https://www.uctronics.com/arducam-64mp-auto-focus-quad-camera-kit.html</t>
+  </si>
+  <si>
+    <t>https://www.uctronics.com/16mp%20synchronized%20quad-camera%20kit.html</t>
+  </si>
+  <si>
+    <t>https://www.uctronics.com/arducam-1mp-4-quadrascopic-camera-bundle-kit-imx219-raspberry%20pi-nvidia-jetson-nano-xavier-nx,.html</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4b 4GB</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/4296</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4b 2GB</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/4295</t>
+  </si>
+  <si>
+    <t>PiSugar3 Plus</t>
+  </si>
+  <si>
+    <t>https://a.co/d/1oStHeO</t>
+  </si>
+  <si>
+    <t>PiSugar2 Plus</t>
+  </si>
+  <si>
+    <t>https://a.co/d/bhYGM9O</t>
+  </si>
+  <si>
+    <t>PiSugar S Pro</t>
+  </si>
+  <si>
+    <t>https://a.co/d/dbIsF8b</t>
+  </si>
+  <si>
+    <t>Video Version</t>
   </si>
   <si>
     <t>https://www.uctronics.com/camera-modules/camera-for-raspberry-pi/16mp%20synchronized%20quad-camera%20kit.html</t>
   </si>
   <si>
-    <t>https://www.uctronics.com/camera-modules/camera-for-raspberry-pi/arducam-1mp-4-quadrascopic-camera-bundle-kit-imx219-raspberry%20pi-nvidia-jetson-nano-xavier-nx,.html</t>
-  </si>
-  <si>
-    <t>Raspberry Pi 4b 4GB</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/4296</t>
-  </si>
-  <si>
-    <t>Raspberry Pi 4b 2GB</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/4295</t>
-  </si>
-  <si>
-    <t>PiSugar3 Plus</t>
-  </si>
-  <si>
-    <t>https://a.co/d/1oStHeO</t>
-  </si>
-  <si>
-    <t>PiSugar2 Plus</t>
-  </si>
-  <si>
-    <t>https://a.co/d/bhYGM9O</t>
-  </si>
-  <si>
-    <t>PiSugar S Pro</t>
-  </si>
-  <si>
-    <t>https://a.co/d/dbIsF8b</t>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Mini Cam Arduino Version</t>
+  </si>
+  <si>
+    <t>Camarry HAT</t>
+  </si>
+  <si>
+    <t>https://www.uctronics.com/arducam-mini-multi-camera-adapter-board-for-arduino-raspberry-pi.html</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Zero</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2885</t>
+  </si>
+  <si>
+    <t>4x 5MP Cameras</t>
+  </si>
+  <si>
+    <t>https://www.uctronics.com/arducam-mini-module-camera-shield-5mp-plus-ov5642-camera-module-for-arduino-uno-mega-2560-board.html</t>
+  </si>
+  <si>
+    <t>Jumper Wires</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://www.ebay.com/itm/323880837276</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://a.co/d/1mBlzoZ</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve"> or maybe </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://a.co/d/2VHOSsp</t>
+    </r>
+  </si>
+  <si>
+    <t>PiSugar 3</t>
+  </si>
+  <si>
+    <t>https://www.tindie.com/products/pisugar/pisugar-3-battery-for-raspberry-pi-zero/</t>
+  </si>
+  <si>
+    <t>Professional Version</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Camarray HAT &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> 6 Cameras</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.arducam.com/product/arducam-imx219-multi-camera-kit-for-the-nvidia-jetson-agx-orin/</t>
+  </si>
+  <si>
+    <t>Nvidia Jetson AGX Orin</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/NVIDIA-Jetson-Orin-64GB-Developer/dp/B0BYGB3WV4/ref=sr_1_2?keywords=Nvidia+Jetson+AGX+orin&amp;s=electronics&amp;sr=1-2</t>
   </si>
   <si>
     <t>Can I rebuild this 40 year old 3D camera into a digital one?</t>
@@ -74,10 +170,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -115,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -129,6 +231,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -404,7 +510,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.38"/>
+    <col customWidth="1" min="1" max="1" width="20.63"/>
     <col customWidth="1" min="2" max="2" width="25.38"/>
     <col customWidth="1" min="3" max="3" width="93.63"/>
     <col customWidth="1" min="5" max="5" width="113.63"/>
@@ -422,107 +528,242 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>320.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2">
+        <v>300.0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2">
+        <v>170.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
+        <v>140.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>55.0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>45.0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2">
         <v>170.0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>139.0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2">
+        <v>55.0</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1">
-        <v>55.0</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1">
-        <v>45.0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1">
+    </row>
+    <row r="23">
+      <c r="A23" s="2">
         <v>50.0</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1">
-        <v>50.0</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>17</v>
+    </row>
+    <row r="25">
+      <c r="A25" s="5">
+        <f>SUM(A21:A24)</f>
+        <v>275</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2">
+        <v>160.0</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5">
+        <f>(SUM(A30:A34))</f>
+        <v>255</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2">
+        <v>180.0</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="45">
-      <c r="E45" s="4" t="s">
-        <v>18</v>
+      <c r="E45" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -530,14 +771,23 @@
     <hyperlink r:id="rId1" ref="C2"/>
     <hyperlink r:id="rId2" ref="C3"/>
     <hyperlink r:id="rId3" ref="C4"/>
-    <hyperlink r:id="rId4" ref="C5"/>
+    <hyperlink r:id="rId4" ref="C8"/>
     <hyperlink r:id="rId5" ref="C9"/>
-    <hyperlink r:id="rId6" ref="C10"/>
+    <hyperlink r:id="rId6" ref="C13"/>
     <hyperlink r:id="rId7" ref="C14"/>
     <hyperlink r:id="rId8" ref="C15"/>
-    <hyperlink r:id="rId9" ref="C16"/>
-    <hyperlink r:id="rId10" ref="E45"/>
+    <hyperlink r:id="rId9" ref="C21"/>
+    <hyperlink r:id="rId10" ref="C22"/>
+    <hyperlink r:id="rId11" ref="C23"/>
+    <hyperlink r:id="rId12" ref="C30"/>
+    <hyperlink r:id="rId13" ref="C31"/>
+    <hyperlink r:id="rId14" ref="C32"/>
+    <hyperlink r:id="rId15" ref="C33"/>
+    <hyperlink r:id="rId16" ref="C34"/>
+    <hyperlink r:id="rId17" ref="C41"/>
+    <hyperlink r:id="rId18" ref="C42"/>
+    <hyperlink r:id="rId19" ref="E45"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Parts List and README
</commit_message>
<xml_diff>
--- a/Parts List - Digital Nishika N8000.xlsx
+++ b/Parts List - Digital Nishika N8000.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Price</t>
   </si>
@@ -67,13 +67,22 @@
     <t>Video Version</t>
   </si>
   <si>
+    <t>Can I rebuild this 40 year old 3D camera into a digital one?</t>
+  </si>
+  <si>
     <t>https://www.uctronics.com/camera-modules/camera-for-raspberry-pi/16mp%20synchronized%20quad-camera%20kit.html</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Mini Cam Arduino Version</t>
+    <t>↓↓↓↓↓↓↓↓↓↓↓</t>
+  </si>
+  <si>
+    <t>BUY THESE</t>
+  </si>
+  <si>
+    <t>Mini Cam PiZero Version</t>
   </si>
   <si>
     <t>Camarry HAT</t>
@@ -89,12 +98,6 @@
   </si>
   <si>
     <t>4x 5MP Cameras</t>
-  </si>
-  <si>
-    <t>https://www.uctronics.com/arducam-mini-module-camera-shield-5mp-plus-ov5642-camera-module-for-arduino-uno-mega-2560-board.html</t>
-  </si>
-  <si>
-    <t>Jumper Wires</t>
   </si>
   <si>
     <r>
@@ -102,10 +105,12 @@
         <color rgb="FF1155CC"/>
         <u/>
       </rPr>
-      <t>https://www.ebay.com/itm/323880837276</t>
+      <t>https://www.uctronics.com/arducam-mini-module-camera-shield-5mp-plus-ov5642-camera-module-for-arduino-uno-mega-2560-board.html</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <color rgb="FF000000"/>
+      </rPr>
       <t xml:space="preserve"> or </t>
     </r>
     <r>
@@ -113,19 +118,8 @@
         <color rgb="FF1155CC"/>
         <u/>
       </rPr>
-      <t>https://a.co/d/1mBlzoZ</t>
+      <t>https://www.uctronics.com/camera-modules/camera-for-arduino/arducam-mini-module-camera-shield-w-2-mp-ov2640-for-arduino-uno-mega2560-board.html</t>
     </r>
-    <r>
-      <rPr/>
-      <t xml:space="preserve"> or maybe </t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://a.co/d/2VHOSsp</t>
-    </r>
   </si>
   <si>
     <t>PiSugar 3</t>
@@ -134,43 +128,23 @@
     <t>https://www.tindie.com/products/pisugar/pisugar-3-battery-for-raspberry-pi-zero/</t>
   </si>
   <si>
-    <t>Professional Version</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>Camarray HAT &amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> 6 Cameras</t>
-    </r>
-  </si>
-  <si>
-    <t>https://www.arducam.com/product/arducam-imx219-multi-camera-kit-for-the-nvidia-jetson-agx-orin/</t>
-  </si>
-  <si>
-    <t>Nvidia Jetson AGX Orin</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/NVIDIA-Jetson-Orin-64GB-Developer/dp/B0BYGB3WV4/ref=sr_1_2?keywords=Nvidia+Jetson+AGX+orin&amp;s=electronics&amp;sr=1-2</t>
-  </si>
-  <si>
-    <t>Can I rebuild this 40 year old 3D camera into a digital one?</t>
+    <t>CamArray Pins</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2822</t>
+  </si>
+  <si>
+    <t>Right Angle Pin Header</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2823</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -202,13 +176,37 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="26.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="27.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -217,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -233,8 +231,17 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -257,7 +264,7 @@
     <xdr:ext cx="7324725" cy="4124325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -277,10 +284,38 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7620000" cy="7620000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="8105775" cy="4124325"/>
     <xdr:pic>
@@ -289,7 +324,7 @@
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -510,7 +545,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.63"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
     <col customWidth="1" min="2" max="2" width="25.38"/>
     <col customWidth="1" min="3" max="3" width="93.63"/>
     <col customWidth="1" min="5" max="5" width="113.63"/>
@@ -622,6 +657,9 @@
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C20" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
@@ -631,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -657,17 +695,28 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="5">
+      <c r="A25" s="6">
         <f>SUM(A21:A24)</f>
         <v>275</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" ht="69.75" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30">
@@ -675,10 +724,10 @@
         <v>15.0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31">
@@ -686,10 +735,10 @@
         <v>20.0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
@@ -697,74 +746,56 @@
         <v>160.0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <v>40.0</v>
+        <v>1.0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="5">
-        <f>(SUM(A30:A34))</f>
-        <v>255</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6">
+        <f>(SUM(A30:A35))</f>
+        <v>237.5</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="2">
-        <v>180.0</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="2">
-        <v>2000.0</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="E45" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A40" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -776,18 +807,17 @@
     <hyperlink r:id="rId6" ref="C13"/>
     <hyperlink r:id="rId7" ref="C14"/>
     <hyperlink r:id="rId8" ref="C15"/>
-    <hyperlink r:id="rId9" ref="C21"/>
-    <hyperlink r:id="rId10" ref="C22"/>
-    <hyperlink r:id="rId11" ref="C23"/>
-    <hyperlink r:id="rId12" ref="C30"/>
-    <hyperlink r:id="rId13" ref="C31"/>
-    <hyperlink r:id="rId14" ref="C32"/>
-    <hyperlink r:id="rId15" ref="C33"/>
-    <hyperlink r:id="rId16" ref="C34"/>
-    <hyperlink r:id="rId17" ref="C41"/>
-    <hyperlink r:id="rId18" ref="C42"/>
-    <hyperlink r:id="rId19" ref="E45"/>
+    <hyperlink r:id="rId9" ref="C20"/>
+    <hyperlink r:id="rId10" ref="C21"/>
+    <hyperlink r:id="rId11" ref="C22"/>
+    <hyperlink r:id="rId12" ref="C23"/>
+    <hyperlink r:id="rId13" ref="C30"/>
+    <hyperlink r:id="rId14" ref="C31"/>
+    <hyperlink r:id="rId15" ref="C32"/>
+    <hyperlink r:id="rId16" ref="C33"/>
+    <hyperlink r:id="rId17" ref="C34"/>
+    <hyperlink r:id="rId18" ref="C35"/>
   </hyperlinks>
-  <drawing r:id="rId20"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>